<commit_message>
template improvements for Excel processing
</commit_message>
<xml_diff>
--- a/VocExcel-template.xlsx
+++ b/VocExcel-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/surround/VocExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BF5E54-98C9-2C49-8720-B978D26D82C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7A2091-9DE5-DA48-B33C-34B51077A299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="500" windowWidth="36460" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="500" windowWidth="36460" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vocabulary" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="131">
   <si>
     <t>When was this vocabulary first created?</t>
   </si>
@@ -431,7 +431,19 @@
     <t>All Concepts in this vocabulary</t>
   </si>
   <si>
-    <t>&lt;http://resource.geosciml.org/classifier/cgi/particletype/accidental_pyroclastic_fragment,
+    <t>This example shows an incomplete vocabulary with a Concept hierarchy and a Collection</t>
+  </si>
+  <si>
+    <t>eCat DOI</t>
+  </si>
+  <si>
+    <t>http://resource.geosciml.org/classifierscheme/cgi/2016.01/particletype</t>
+  </si>
+  <si>
+    <t>one, two,three</t>
+  </si>
+  <si>
+    <t>http://resource.geosciml.org/classifier/cgi/particletype/accidental_pyroclastic_fragment,
 http://resource.geosciml.org/classifier/cgi/particletype/aggregate_non-clastic_particle,
 http://resource.geosciml.org/classifier/cgi/particletype/amygdule,
 http://resource.geosciml.org/classifier/cgi/particletype/autoclast,
@@ -459,8 +471,7 @@
 http://resource.geosciml.org/classifier/cgi/particletype/hydroclast,
 http://resource.geosciml.org/classifier/cgi/particletype/hydrothermal_vein,
 http://resource.geosciml.org/classifier/cgi/particletype/igneous_inclusion,
-http://resource.geosciml.org/classifier/cgi/particletype/igneous_vein,
-http://resource.geosciml.org/classifier/cgi/particletype/intraclast,
+http://resource.geosciml.org/classifier/cgi/particletype/igneous_vein,http://resource.geosciml.org/classifier/cgi/particletype/intraclast,
 http://resource.geosciml.org/classifier/cgi/particletype/intrusive_sheet,
 http://resource.geosciml.org/classifier/cgi/particletype/juvenile_pyroclastic_fragment,
 http://resource.geosciml.org/classifier/cgi/particletype/lithic_clast,
@@ -495,16 +506,13 @@
 http://resource.geosciml.org/classifier/cgi/particletype/xenocryst&gt;</t>
   </si>
   <si>
-    <t>This example shows an incomplete vocabulary with a Concept hierarchy and a Collection</t>
-  </si>
-  <si>
-    <t>http://resource.geos$ciml.org/classifierscheme/cgi/2016.01/particletype</t>
-  </si>
-  <si>
-    <t>eCat DOI</t>
-  </si>
-  <si>
-    <t>GA's catalogue DOI, if the vocab has one</t>
+    <t>http://pid.geoscience.gov.au/dataset/ga/114541</t>
+  </si>
+  <si>
+    <t>Catalogue ID</t>
+  </si>
+  <si>
+    <t>A catalogue PID or DOI, e.g. eCat ID,, if the vocab has one</t>
   </si>
 </sst>
 </file>
@@ -600,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -687,6 +695,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1029,15 +1040,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="51.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="58.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="28.6640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="3" customWidth="1"/>
@@ -1159,10 +1170,10 @@
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>54</v>
@@ -1202,7 +1213,7 @@
         <v>92</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1241,7 +1252,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1374,6 +1385,11 @@
         <v>57</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>34</v>
@@ -1532,17 +1548,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ADB3B5-8C0A-3A40-96EE-C1A713CE0AB4}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="59.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.1640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="47" style="16" customWidth="1"/>
     <col min="4" max="4" width="62.1640625" style="11" customWidth="1"/>
     <col min="5" max="5" width="28.6640625" style="11" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="16" customWidth="1"/>
@@ -1687,112 +1703,126 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
-        <v>120</v>
-      </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E15" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F15" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G15" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H15" s="19" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B26" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C26" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E26" s="19" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1804,29 +1834,30 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{443668A0-E6EF-8346-8B22-73120CCB3DD1}"/>
-    <hyperlink ref="A15" r:id="rId2" xr:uid="{CBF8F826-C7B2-0F4D-A5F0-C4A2EE95BF7A}"/>
-    <hyperlink ref="A16" r:id="rId3" xr:uid="{8E92FF6C-228F-0840-8350-DC539566208E}"/>
-    <hyperlink ref="A17" r:id="rId4" xr:uid="{C211815B-DD22-1A4C-BDD3-CC5865EE4E55}"/>
-    <hyperlink ref="A18" r:id="rId5" xr:uid="{1F39F9AF-A383-2E4D-9DA2-CB233B35AB29}"/>
-    <hyperlink ref="A19" r:id="rId6" xr:uid="{EB4CF36F-BD37-1745-A32C-6279BF083AC1}"/>
+    <hyperlink ref="A16" r:id="rId2" xr:uid="{CBF8F826-C7B2-0F4D-A5F0-C4A2EE95BF7A}"/>
+    <hyperlink ref="A17" r:id="rId3" xr:uid="{8E92FF6C-228F-0840-8350-DC539566208E}"/>
+    <hyperlink ref="A18" r:id="rId4" xr:uid="{C211815B-DD22-1A4C-BDD3-CC5865EE4E55}"/>
+    <hyperlink ref="A19" r:id="rId5" xr:uid="{1F39F9AF-A383-2E4D-9DA2-CB233B35AB29}"/>
+    <hyperlink ref="A20" r:id="rId6" xr:uid="{EB4CF36F-BD37-1745-A32C-6279BF083AC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9506A97D-B28B-2944-8448-271454E088D2}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D11" sqref="C11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="59.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46" style="3" customWidth="1"/>
     <col min="4" max="4" width="74" style="4" customWidth="1"/>
     <col min="5" max="5" width="55.1640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="3" customWidth="1"/>
@@ -1839,7 +1870,7 @@
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="35" t="s">
         <v>125</v>
       </c>
       <c r="C1" s="9" t="s">
@@ -1924,7 +1955,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>50</v>
@@ -1975,140 +2006,154 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
-        <v>124</v>
-      </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+    <row r="16" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="A16" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="C16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="H16" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="128" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>118</v>
-      </c>
+      <c r="E17" s="3"/>
       <c r="H17" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
-    </row>
-    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="31"/>
+    </row>
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:8" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2119,7 +2164,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A15" r:id="rId1" xr:uid="{1D8500EE-16B8-C047-9B8C-221632D7BA36}"/>
+    <hyperlink ref="A16" r:id="rId1" xr:uid="{1D8500EE-16B8-C047-9B8C-221632D7BA36}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{CC8F6245-2EDC-B74C-AB53-EC08C2B8EE5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2130,7 +2176,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2209,5 +2255,6 @@
     <hyperlink ref="B5" r:id="rId5" xr:uid="{650CC3D1-9C0E-244A-BD7A-2B992E1A1C0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
conversion working; output formats selectable
</commit_message>
<xml_diff>
--- a/VocExcel-template.xlsx
+++ b/VocExcel-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/surround/VocExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7A2091-9DE5-DA48-B33C-34B51077A299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB62689-0FC2-624A-A54A-4C51D951AF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="500" windowWidth="36460" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="500" windowWidth="36460" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vocabulary" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="example - simple" sheetId="5" r:id="rId3"/>
     <sheet name="example - complex" sheetId="7" r:id="rId4"/>
     <sheet name="lists" sheetId="4" r:id="rId5"/>
+    <sheet name="program info" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Publishers">lists!$A$2:$A$6</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="139">
   <si>
     <t>When was this vocabulary first created?</t>
   </si>
@@ -434,13 +435,31 @@
     <t>This example shows an incomplete vocabulary with a Concept hierarchy and a Collection</t>
   </si>
   <si>
-    <t>eCat DOI</t>
-  </si>
-  <si>
     <t>http://resource.geosciml.org/classifierscheme/cgi/2016.01/particletype</t>
   </si>
   <si>
     <t>one, two,three</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/dataset/ga/114541</t>
+  </si>
+  <si>
+    <t>A catalogue PID or DOI, e.g. eCat ID,, if the vocab has one</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>VocExcel</t>
+  </si>
+  <si>
+    <t>Code Repository</t>
+  </si>
+  <si>
+    <t>https://github.com/surroundaustralia/VocExcel</t>
+  </si>
+  <si>
+    <t>Catalogue PID</t>
   </si>
   <si>
     <t>http://resource.geosciml.org/classifier/cgi/particletype/accidental_pyroclastic_fragment,
@@ -503,16 +522,22 @@
 http://resource.geosciml.org/classifier/cgi/particletype/ventrifact,
 http://resource.geosciml.org/classifier/cgi/particletype/vesicle,
 http://resource.geosciml.org/classifier/cgi/particletype/vug,
-http://resource.geosciml.org/classifier/cgi/particletype/xenocryst&gt;</t>
-  </si>
-  <si>
-    <t>http://pid.geoscience.gov.au/dataset/ga/114541</t>
-  </si>
-  <si>
-    <t>Catalogue ID</t>
-  </si>
-  <si>
-    <t>A catalogue PID or DOI, e.g. eCat ID,, if the vocab has one</t>
+http://resource.geosciml.org/classifier/cgi/particletype/xenocryst</t>
+  </si>
+  <si>
+    <t>http://resource.geosciml.org/classifier/cgi/particletype/vug</t>
+  </si>
+  <si>
+    <t>vug</t>
+  </si>
+  <si>
+    <t>Irregular cavity in rock, generic term with no connotation of origin of cavity. May be lined with crystals of different mineral compostion to the host rock</t>
+  </si>
+  <si>
+    <t>http://resource.geosciml.org/classifier/cgi/particletype/miarolitic_cavity</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
   </si>
 </sst>
 </file>
@@ -608,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -695,9 +720,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1041,7 +1063,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1078,7 +1100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -1170,10 +1192,10 @@
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>54</v>
@@ -1251,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29D9D1C-A589-F545-B75A-0C9180A707C5}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1384,10 +1406,19 @@
       <c r="B14" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>124</v>
+        <v>132</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1480,6 +1511,9 @@
       </c>
       <c r="B25" s="32" t="s">
         <v>111</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1550,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ADB3B5-8C0A-3A40-96EE-C1A713CE0AB4}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1594,7 +1628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -1705,13 +1739,13 @@
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>54</v>
@@ -1849,29 +1883,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9506A97D-B28B-2944-8448-271454E088D2}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="C11:D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="59.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="46" style="3" customWidth="1"/>
     <col min="4" max="4" width="74" style="4" customWidth="1"/>
-    <col min="5" max="5" width="55.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="57.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>125</v>
+      <c r="B1" s="31" t="s">
+        <v>124</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>4</v>
@@ -2008,10 +2042,10 @@
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>54</v>
@@ -2054,15 +2088,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+    <row r="16" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>109</v>
@@ -2120,8 +2154,19 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
+    <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -2151,7 +2196,7 @@
         <v>122</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>116</v>
@@ -2166,8 +2211,10 @@
   <hyperlinks>
     <hyperlink ref="A16" r:id="rId1" xr:uid="{1D8500EE-16B8-C047-9B8C-221632D7BA36}"/>
     <hyperlink ref="B1" r:id="rId2" xr:uid="{CC8F6245-2EDC-B74C-AB53-EC08C2B8EE5D}"/>
+    <hyperlink ref="E20" r:id="rId3" display="http://cgi.vocabs.ga.gov.au/object?uri=http%3A//resource.geosciml.org/classifier/cgi/particletype/miarolitic_cavity" xr:uid="{CEF8010D-BA18-484E-8730-BD1E6F87EF59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2257,4 +2304,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E95ED1A-35C6-6345-A556-6100B889990F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update Excel template inline with VocPub profile
</commit_message>
<xml_diff>
--- a/VocExcel-template.xlsx
+++ b/VocExcel-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/surround/VocExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB62689-0FC2-624A-A54A-4C51D951AF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EE21DA-27A5-8B4E-A97B-8FBEB286D4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="500" windowWidth="36460" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2060" yWindow="500" windowWidth="36340" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vocabulary" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="141">
   <si>
     <t>When was this vocabulary first created?</t>
   </si>
@@ -538,6 +538,12 @@
   </si>
   <si>
     <t>0.2.1</t>
+  </si>
+  <si>
+    <t>required: selected from drop-down list</t>
+  </si>
+  <si>
+    <t>A catalogue PID or DOI, e.g. eCat ID, if the vocab has one</t>
   </si>
 </sst>
 </file>
@@ -1063,14 +1069,14 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="51.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="46.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="58.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="28.6640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="3" customWidth="1"/>
@@ -1143,7 +1149,7 @@
         <v>50</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1154,7 +1160,7 @@
         <v>50</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1176,7 +1182,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1195,7 +1201,7 @@
         <v>132</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>54</v>
@@ -1273,7 +1279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29D9D1C-A589-F545-B75A-0C9180A707C5}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1928,7 +1934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2123,7 +2129,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
@@ -2310,7 +2316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E95ED1A-35C6-6345-A556-6100B889990F}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
multi-lingual preflabel and definition support for Concepts
</commit_message>
<xml_diff>
--- a/VocExcel-template.xlsx
+++ b/VocExcel-template.xlsx
@@ -8,38 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/surround/VocExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EE21DA-27A5-8B4E-A97B-8FBEB286D4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F316A-2F32-A14C-9FD5-DAC0F0EE6EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="36340" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="500" windowWidth="36000" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vocabulary" sheetId="2" r:id="rId1"/>
     <sheet name="notes" sheetId="6" r:id="rId2"/>
     <sheet name="example - simple" sheetId="5" r:id="rId3"/>
     <sheet name="example - complex" sheetId="7" r:id="rId4"/>
-    <sheet name="lists" sheetId="4" r:id="rId5"/>
-    <sheet name="program info" sheetId="8" r:id="rId6"/>
+    <sheet name="example - multilang" sheetId="9" r:id="rId5"/>
+    <sheet name="lists" sheetId="4" r:id="rId6"/>
+    <sheet name="program info" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Publishers">lists!$A$2:$A$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="183">
   <si>
     <t>When was this vocabulary first created?</t>
   </si>
@@ -367,9 +357,6 @@
   </si>
   <si>
     <t>bioclast</t>
-  </si>
-  <si>
-    <t>Source</t>
   </si>
   <si>
     <t>NADM SLTTs 2004</t>
@@ -537,13 +524,145 @@
     <t>http://resource.geosciml.org/classifier/cgi/particletype/miarolitic_cavity</t>
   </si>
   <si>
-    <t>0.2.1</t>
-  </si>
-  <si>
     <t>required: selected from drop-down list</t>
   </si>
   <si>
     <t>A catalogue PID or DOI, e.g. eCat ID, if the vocab has one</t>
+  </si>
+  <si>
+    <t>The International Standard ISO3166 is used to determine the codes of letters and/or numbers when referring electronically to countries and their subdivisions.</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/def/voc/ga/countrycode</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>https://www.iso.org/obp/ui/#iso:code:3166:CA</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/def/voc/ga/countrycode/CA-PE</t>
+  </si>
+  <si>
+    <t>Prince Edward Island</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/def/voc/ga/countrycode/CA-QC</t>
+  </si>
+  <si>
+    <t>Quebec</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/def/voc/ga/countrycode/CA-SK</t>
+  </si>
+  <si>
+    <t>Saskatchewan</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/def/voc/ga/countrycode/CA-YT</t>
+  </si>
+  <si>
+    <t>Yukon</t>
+  </si>
+  <si>
+    <t>https://www.iso.org/obp/ui/#iso:code:3166:NZ</t>
+  </si>
+  <si>
+    <t>mri</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/def/voc/ga/countrycode/NZ-HKB</t>
+  </si>
+  <si>
+    <t>Hawke's Bay</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/def/voc/ga/countrycode/NZ-MBH</t>
+  </si>
+  <si>
+    <t>Marlborough</t>
+  </si>
+  <si>
+    <t>Te Tauihu-o-te-waka</t>
+  </si>
+  <si>
+    <t>http://pid.geoscience.gov.au/def/voc/ga/countrycode/NZ-MWT</t>
+  </si>
+  <si>
+    <t>Manawatu Whanganui</t>
+  </si>
+  <si>
+    <t>Manawatu-Wanganui</t>
+  </si>
+  <si>
+    <t>GA Country Code</t>
+  </si>
+  <si>
+    <t>GA Country Codes are ISO3166 compliant country and sub-division codes as used by GA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSmith, DPI </t>
+  </si>
+  <si>
+    <t>These codes are sourced from https://www.iso.org/obp/</t>
+  </si>
+  <si>
+    <t>Te Matau a Maui</t>
+  </si>
+  <si>
+    <t>Île-du-Prince-Édouard</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>Definition Language Code</t>
+  </si>
+  <si>
+    <t>Preferred Label Language code</t>
+  </si>
+  <si>
+    <t>Preferred Label Language Code</t>
+  </si>
+  <si>
+    <t>Optional, default is eng</t>
+  </si>
+  <si>
+    <t>ISO 639-2 or 639-3 two or three letter language code for the Definition.
+To create a Concept with multiple Definitions in different languages, repeat the entire Concept row in Excel and change only the Definition and the Definition Language Code. See example - multilang Worksheet for an example.</t>
+  </si>
+  <si>
+    <t>CA-PE</t>
+  </si>
+  <si>
+    <t>CA-QC</t>
+  </si>
+  <si>
+    <t>CA-SK</t>
+  </si>
+  <si>
+    <t>CA-YT</t>
+  </si>
+  <si>
+    <t>NZ-HKB</t>
+  </si>
+  <si>
+    <t>NZ-MBH</t>
+  </si>
+  <si>
+    <t>NZ-MWT</t>
+  </si>
+  <si>
+    <t>eng,fra</t>
+  </si>
+  <si>
+    <t>ISO 639-2 or 639-3 two or three letter language code for the Preferred Label.
+To create a Concept with multiple Preferred Labels in different languages, repeat the entire Concept row in Excel and change only the Preferred Label and the Preferred Lanble Language Code. See example - multilang Worksheet for an example.
+To assign multiple langage labels to the You may comma-separate multiple language labels if multiple apply to the same term e.g. for the Canadian province Yukno, you may indicate eng,fra to have "Yukno"@eng &amp; "Yukon"@fra.</t>
   </si>
 </sst>
 </file>
@@ -553,7 +672,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,6 +721,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -639,7 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -698,9 +824,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -727,6 +850,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1065,208 +1226,259 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC276"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="30.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="56.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="36" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" style="36" customWidth="1"/>
+    <col min="6" max="6" width="21" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61" style="36" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="39" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="39" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="39" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D6" s="39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D7" s="39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="39" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="39" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+    </row>
+    <row r="15" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="H15" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="I15" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="J15" s="44" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="E19" s="34"/>
+      <c r="G19" s="42"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B21" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C21" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D21" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E21" s="40" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="276" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A276" s="3"/>
+      <c r="B276" s="36"/>
+      <c r="C276" s="36"/>
+      <c r="D276" s="36"/>
+      <c r="E276" s="36"/>
+      <c r="F276" s="36"/>
+      <c r="G276" s="36"/>
+      <c r="H276" s="3"/>
+      <c r="I276" s="36"/>
+      <c r="J276" s="3"/>
+      <c r="K276" s="3"/>
+      <c r="L276" s="3"/>
+      <c r="M276" s="3"/>
+      <c r="N276" s="3"/>
+      <c r="O276" s="3"/>
+      <c r="P276" s="3"/>
+      <c r="Q276" s="3"/>
+      <c r="R276" s="3"/>
+      <c r="S276" s="3"/>
+      <c r="T276" s="3"/>
+      <c r="U276" s="3"/>
+      <c r="V276" s="3"/>
+      <c r="W276" s="3"/>
+      <c r="X276" s="3"/>
+      <c r="Y276" s="3"/>
+      <c r="Z276" s="3"/>
+      <c r="AA276" s="3"/>
+      <c r="AB276" s="3"/>
+      <c r="AC276" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{02E6AD3D-0807-F94E-9FD6-D02DC589EDA2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Publishers</formula1>
     </dataValidation>
   </dataValidations>
@@ -1276,18 +1488,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29D9D1C-A589-F545-B75A-0C9180A707C5}">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="86.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -1297,163 +1509,172 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+    <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>24</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>109</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>110</v>
+        <v>51</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>57</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>57</v>
+        <v>131</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-    </row>
-    <row r="18" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+    </row>
+    <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>81</v>
+        <v>27</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>45</v>
+    <row r="19" spans="1:3" ht="124" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -1478,23 +1699,23 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="35" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>48</v>
@@ -1502,58 +1723,58 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>111</v>
+        <v>92</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
-        <v>26</v>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>45</v>
@@ -1561,23 +1782,34 @@
     </row>
     <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B33" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1587,30 +1819,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ADB3B5-8C0A-3A40-96EE-C1A713CE0AB4}">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="59.6640625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.1640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="47" style="16" customWidth="1"/>
-    <col min="4" max="4" width="62.1640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="30.5" style="16" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="16"/>
+    <col min="4" max="4" width="34.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="17" t="s">
@@ -1620,7 +1855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -1634,7 +1869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -1648,7 +1883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>40</v>
       </c>
@@ -1662,7 +1897,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>41</v>
       </c>
@@ -1676,7 +1911,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
@@ -1690,7 +1925,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1704,7 +1939,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
@@ -1715,7 +1950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>25</v>
       </c>
@@ -1729,7 +1964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>51</v>
       </c>
@@ -1743,113 +1978,132 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
-        <v>120</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>119</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
     </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="E15" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="F15" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="G15" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="H15" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="I15" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
+      <c r="J15" s="43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
         <v>82</v>
       </c>
       <c r="B16" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="16"/>
+      <c r="F16" s="11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="47" t="s">
         <v>83</v>
       </c>
       <c r="B17" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="16"/>
+      <c r="F17" s="11" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="47" t="s">
         <v>84</v>
       </c>
       <c r="B18" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="16"/>
+      <c r="F18" s="11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="47" t="s">
         <v>85</v>
       </c>
       <c r="B19" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="16"/>
+      <c r="F19" s="11" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="47" t="s">
         <v>86</v>
       </c>
       <c r="B20" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="16"/>
+      <c r="F20" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="46"/>
+    </row>
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>32</v>
       </c>
@@ -1868,17 +2122,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{2CCF9A47-B0DF-4F4B-A403-9BBC3CC2275A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>Publishers</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{443668A0-E6EF-8346-8B22-73120CCB3DD1}"/>
-    <hyperlink ref="A16" r:id="rId2" xr:uid="{CBF8F826-C7B2-0F4D-A5F0-C4A2EE95BF7A}"/>
-    <hyperlink ref="A17" r:id="rId3" xr:uid="{8E92FF6C-228F-0840-8350-DC539566208E}"/>
-    <hyperlink ref="A18" r:id="rId4" xr:uid="{C211815B-DD22-1A4C-BDD3-CC5865EE4E55}"/>
-    <hyperlink ref="A19" r:id="rId5" xr:uid="{1F39F9AF-A383-2E4D-9DA2-CB233B35AB29}"/>
-    <hyperlink ref="A20" r:id="rId6" xr:uid="{EB4CF36F-BD37-1745-A32C-6279BF083AC1}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1886,32 +2135,34 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9506A97D-B28B-2944-8448-271454E088D2}">
-  <dimension ref="A1:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="59.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="46" style="3" customWidth="1"/>
-    <col min="4" max="4" width="74" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="72.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="3"/>
+    <col min="9" max="9" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>124</v>
+      <c r="B1" s="30" t="s">
+        <v>123</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>4</v>
@@ -1920,7 +2171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
@@ -1934,7 +2185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -1948,11 +2199,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="29">
         <v>40008</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -1962,11 +2213,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="29">
         <v>44005</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1976,7 +2227,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
@@ -1990,7 +2241,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -2004,7 +2255,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -2018,7 +2269,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -2032,7 +2283,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>51</v>
       </c>
@@ -2046,135 +2297,160 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
-        <v>123</v>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>122</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="G16" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="H17" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>119</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="G18" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="G19" s="4"/>
+      <c r="J19" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="G20" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -2191,33 +2467,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{94361002-7066-F448-8DC2-07D5E5CB74AD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>Publishers</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A16" r:id="rId1" xr:uid="{1D8500EE-16B8-C047-9B8C-221632D7BA36}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{CC8F6245-2EDC-B74C-AB53-EC08C2B8EE5D}"/>
-    <hyperlink ref="E20" r:id="rId3" display="http://cgi.vocabs.ga.gov.au/object?uri=http%3A//resource.geosciml.org/classifier/cgi/particletype/miarolitic_cavity" xr:uid="{CEF8010D-BA18-484E-8730-BD1E6F87EF59}"/>
+    <hyperlink ref="A16" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="G20" r:id="rId3" display="http://cgi.vocabs.ga.gov.au/object?uri=http%3A//resource.geosciml.org/classifier/cgi/particletype/miarolitic_cavity" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2225,17 +2501,561 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3748346F-E4CF-E548-BC40-4CCE831AF1DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BC6D4A-EE88-EF4C-B47B-08A2B35F3812}">
+  <dimension ref="A1:J34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="36" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" style="36" customWidth="1"/>
+    <col min="6" max="6" width="21" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.6640625" style="36" customWidth="1"/>
+    <col min="8" max="8" width="16" style="35" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.5" style="35" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="41">
+        <v>44139</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="41">
+        <v>44453</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="36">
+        <v>2</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+    </row>
+    <row r="15" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A16" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H16" s="36"/>
+      <c r="I16" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="J16" s="36"/>
+    </row>
+    <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" s="36"/>
+      <c r="I17" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="J17" s="36"/>
+    </row>
+    <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A18" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H18" s="36"/>
+      <c r="I18" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="J18" s="36"/>
+    </row>
+    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A19" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H19" s="36"/>
+      <c r="I19" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A20" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H20" s="36"/>
+      <c r="I20" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="J20" s="36"/>
+    </row>
+    <row r="21" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A21" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="36"/>
+      <c r="I21" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="J21" s="36"/>
+    </row>
+    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A22" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" s="36"/>
+      <c r="I22" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="J22" s="36"/>
+    </row>
+    <row r="23" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A23" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H23" s="36"/>
+      <c r="I23" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="J23" s="36"/>
+    </row>
+    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="36"/>
+      <c r="I24" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="J24" s="36"/>
+    </row>
+    <row r="25" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A25" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H25" s="36"/>
+      <c r="I25" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="J25" s="36"/>
+    </row>
+    <row r="26" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A26" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H26" s="36"/>
+      <c r="I26" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="J26" s="36"/>
+    </row>
+    <row r="27" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A27" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H27" s="36"/>
+      <c r="I27" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="J27" s="36"/>
+    </row>
+    <row r="28" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A28" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="H28" s="36"/>
+      <c r="I28" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="J28" s="36"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="E32" s="34"/>
+      <c r="G32" s="42"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{71BDF466-626D-DA46-89A6-618460B87383}">
+      <formula1>Publishers</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2301,26 +3121,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{2909EB31-5D80-6742-ADF6-16D709EEE69A}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{5D4BC2AC-F33C-964B-B530-2FD2530AFAC3}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{0080F661-A776-BA47-B66F-8A4D7AB8B3D1}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{E62CE5CF-FD54-444D-A0C2-53F6A271345D}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{650CC3D1-9C0E-244A-BD7A-2B992E1A1C0E}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E95ED1A-35C6-6345-A556-6100B889990F}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
@@ -2328,10 +3148,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
         <v>128</v>
-      </c>
-      <c r="B1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2339,18 +3159,300 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
         <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6D783E0ADD6B749A2702D2B7777A319" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="44cc23be00774fb4854ef8279c035cc3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97bb4d45-1042-4c49-a7f1-494cbdb4d63a" xmlns:ns4="40d17f1d-405e-4b2c-9582-827b4e442104" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8c5d83f61cd4c248c617d7792973ac3" ns3:_="" ns4:_="">
+    <xsd:import namespace="97bb4d45-1042-4c49-a7f1-494cbdb4d63a"/>
+    <xsd:import namespace="40d17f1d-405e-4b2c-9582-827b4e442104"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="97bb4d45-1042-4c49-a7f1-494cbdb4d63a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="40d17f1d-405e-4b2c-9582-827b4e442104" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9AB3520-0A58-4CB2-8628-A79091974E95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="97bb4d45-1042-4c49-a7f1-494cbdb4d63a"/>
+    <ds:schemaRef ds:uri="40d17f1d-405e-4b2c-9582-827b4e442104"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{915D0155-BA4B-44F2-9111-0BC494AB9DE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14FB0D8E-A90D-4B0C-ACC2-9EDC9E6A8195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="97bb4d45-1042-4c49-a7f1-494cbdb4d63a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="40d17f1d-405e-4b2c-9582-827b4e442104"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Relaxed creator & publisher allowed values, updated Excel templates to reflect, fixed Concept children URIs & openpyxl active sheet
</commit_message>
<xml_diff>
--- a/VocExcel-template.xlsx
+++ b/VocExcel-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/surround/VocExcel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jamie\surround\VocExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F316A-2F32-A14C-9FD5-DAC0F0EE6EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8FB453-7B41-486C-AC1F-E2A5531BA09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="500" windowWidth="36000" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22845" yWindow="0" windowWidth="22740" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vocabulary" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="186">
   <si>
     <t>When was this vocabulary first created?</t>
   </si>
@@ -663,6 +663,15 @@
     <t>ISO 639-2 or 639-3 two or three letter language code for the Preferred Label.
 To create a Concept with multiple Preferred Labels in different languages, repeat the entire Concept row in Excel and change only the Preferred Label and the Preferred Lanble Language Code. See example - multilang Worksheet for an example.
 To assign multiple langage labels to the You may comma-separate multiple language labels if multiple apply to the same term e.g. for the Canadian province Yukno, you may indicate eng,fra to have "Yukno"@eng &amp; "Yukon"@fra.</t>
+  </si>
+  <si>
+    <t>DES</t>
+  </si>
+  <si>
+    <t>https://linked.data.gov.au/org/des</t>
+  </si>
+  <si>
+    <t>Department of Environment and Science, Queensland Government</t>
   </si>
 </sst>
 </file>
@@ -1230,25 +1239,25 @@
   <dimension ref="A1:AC276"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="36" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="36" customWidth="1"/>
-    <col min="5" max="5" width="43.83203125" style="36" customWidth="1"/>
+    <col min="1" max="1" width="56.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="36" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="36" customWidth="1"/>
     <col min="6" max="6" width="21" style="36" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61" style="36" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
@@ -1270,7 +1279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>40</v>
       </c>
@@ -1293,7 +1302,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>41</v>
       </c>
@@ -1305,7 +1314,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
@@ -1316,7 +1325,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -1327,7 +1336,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -1338,7 +1347,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>51</v>
       </c>
@@ -1360,7 +1369,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>131</v>
       </c>
@@ -1371,18 +1380,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
     </row>
-    <row r="15" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>31</v>
       </c>
@@ -1414,21 +1423,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="E19" s="34"/>
       <c r="G19" s="42"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>32</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="3"/>
       <c r="B276" s="36"/>
       <c r="C276" s="36"/>
@@ -1477,13 +1486,20 @@
       <c r="AC276" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>Publishers</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6:B7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1495,20 +1511,20 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="86.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="86.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -1516,7 +1532,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>19</v>
       </c>
@@ -1527,7 +1543,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>20</v>
       </c>
@@ -1538,7 +1554,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
@@ -1549,7 +1565,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>40</v>
       </c>
@@ -1560,7 +1576,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>41</v>
       </c>
@@ -1571,7 +1587,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
@@ -1582,7 +1598,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>23</v>
       </c>
@@ -1593,7 +1609,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>24</v>
       </c>
@@ -1604,7 +1620,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>25</v>
       </c>
@@ -1615,7 +1631,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>51</v>
       </c>
@@ -1626,7 +1642,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>131</v>
       </c>
@@ -1637,14 +1653,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>31</v>
       </c>
@@ -1655,7 +1671,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>27</v>
       </c>
@@ -1666,7 +1682,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="124" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="123.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>171</v>
       </c>
@@ -1677,7 +1693,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>28</v>
       </c>
@@ -1688,7 +1704,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>26</v>
       </c>
@@ -1699,7 +1715,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="35" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="35" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>169</v>
       </c>
@@ -1710,7 +1726,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>29</v>
       </c>
@@ -1721,7 +1737,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>30</v>
       </c>
@@ -1732,7 +1748,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>92</v>
       </c>
@@ -1743,7 +1759,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>25</v>
       </c>
@@ -1754,14 +1770,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>32</v>
       </c>
@@ -1769,7 +1785,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>27</v>
       </c>
@@ -1780,7 +1796,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>26</v>
       </c>
@@ -1791,7 +1807,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>33</v>
       </c>
@@ -1802,7 +1818,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>25</v>
       </c>
@@ -1823,25 +1839,25 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.1640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" style="16" customWidth="1"/>
     <col min="3" max="3" width="47" style="16" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="16"/>
+    <col min="10" max="10" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>19</v>
       </c>
@@ -1855,7 +1871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -1869,7 +1885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
@@ -1883,7 +1899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>40</v>
       </c>
@@ -1897,7 +1913,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>41</v>
       </c>
@@ -1911,7 +1927,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
@@ -1925,7 +1941,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1939,7 +1955,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
@@ -1950,7 +1966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>25</v>
       </c>
@@ -1961,10 +1977,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>51</v>
       </c>
@@ -1978,7 +1994,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>131</v>
       </c>
@@ -1992,18 +2008,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>119</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
     </row>
-    <row r="15" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>31</v>
       </c>
@@ -2035,7 +2051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
         <v>82</v>
       </c>
@@ -2048,7 +2064,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
         <v>83</v>
       </c>
@@ -2061,7 +2077,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
         <v>84</v>
       </c>
@@ -2074,7 +2090,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
         <v>85</v>
       </c>
@@ -2087,7 +2103,7 @@
       </c>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="47" t="s">
         <v>86</v>
       </c>
@@ -2100,10 +2116,10 @@
       </c>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="46"/>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>32</v>
       </c>
@@ -2121,16 +2137,23 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{00000000-0002-0000-0200-000000000000}">
-      <formula1>Publishers</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6:B7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2139,25 +2162,25 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="46" style="3" customWidth="1"/>
-    <col min="4" max="4" width="72.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68" style="4" customWidth="1"/>
     <col min="6" max="6" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="3"/>
+    <col min="10" max="10" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
@@ -2171,7 +2194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
@@ -2185,7 +2208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2199,7 +2222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>40</v>
       </c>
@@ -2213,7 +2236,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>41</v>
       </c>
@@ -2227,7 +2250,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
@@ -2241,7 +2264,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -2255,7 +2278,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -2269,7 +2292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -2280,10 +2303,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>51</v>
       </c>
@@ -2297,7 +2320,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>131</v>
       </c>
@@ -2308,18 +2331,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>122</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
@@ -2351,7 +2374,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>94</v>
       </c>
@@ -2374,7 +2397,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>100</v>
       </c>
@@ -2392,7 +2415,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
@@ -2413,7 +2436,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>102</v>
       </c>
@@ -2432,7 +2455,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>133</v>
       </c>
@@ -2450,7 +2473,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -2467,7 +2490,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="408.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>95</v>
       </c>
@@ -2485,11 +2508,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{00000000-0002-0000-0300-000000000000}">
-      <formula1>Publishers</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A16" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
@@ -2497,6 +2515,18 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6:B7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2504,26 +2534,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BC6D4A-EE88-EF4C-B47B-08A2B35F3812}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.33203125" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="36" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="36" customWidth="1"/>
-    <col min="5" max="5" width="43.83203125" style="36" customWidth="1"/>
+    <col min="1" max="1" width="56.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="36" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="36" customWidth="1"/>
     <col min="6" max="6" width="21" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.6640625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="49.7109375" style="36" customWidth="1"/>
     <col min="8" max="8" width="16" style="35" customWidth="1"/>
-    <col min="9" max="9" width="39.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5" style="35" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="35"/>
+    <col min="9" max="9" width="39.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" style="35" customWidth="1"/>
+    <col min="11" max="16384" width="10.85546875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
@@ -2537,7 +2567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
@@ -2551,7 +2581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>21</v>
       </c>
@@ -2565,7 +2595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>40</v>
       </c>
@@ -2579,7 +2609,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>41</v>
       </c>
@@ -2593,7 +2623,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
@@ -2607,7 +2637,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -2621,7 +2651,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -2635,7 +2665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -2649,7 +2679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>51</v>
       </c>
@@ -2663,7 +2693,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>131</v>
       </c>
@@ -2674,18 +2704,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
     </row>
-    <row r="15" spans="1:10" s="45" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>31</v>
       </c>
@@ -2717,7 +2747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>144</v>
       </c>
@@ -2739,7 +2769,7 @@
       </c>
       <c r="J16" s="36"/>
     </row>
-    <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>144</v>
       </c>
@@ -2761,7 +2791,7 @@
       </c>
       <c r="J17" s="36"/>
     </row>
-    <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
         <v>146</v>
       </c>
@@ -2783,7 +2813,7 @@
       </c>
       <c r="J18" s="36"/>
     </row>
-    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>146</v>
       </c>
@@ -2805,7 +2835,7 @@
       </c>
       <c r="J19" s="36"/>
     </row>
-    <row r="20" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>148</v>
       </c>
@@ -2827,7 +2857,7 @@
       </c>
       <c r="J20" s="36"/>
     </row>
-    <row r="21" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>148</v>
       </c>
@@ -2849,7 +2879,7 @@
       </c>
       <c r="J21" s="36"/>
     </row>
-    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>150</v>
       </c>
@@ -2871,7 +2901,7 @@
       </c>
       <c r="J22" s="36"/>
     </row>
-    <row r="23" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>154</v>
       </c>
@@ -2893,7 +2923,7 @@
       </c>
       <c r="J23" s="36"/>
     </row>
-    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
         <v>154</v>
       </c>
@@ -2915,7 +2945,7 @@
       </c>
       <c r="J24" s="36"/>
     </row>
-    <row r="25" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>156</v>
       </c>
@@ -2937,7 +2967,7 @@
       </c>
       <c r="J25" s="36"/>
     </row>
-    <row r="26" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
         <v>156</v>
       </c>
@@ -2959,7 +2989,7 @@
       </c>
       <c r="J26" s="36"/>
     </row>
-    <row r="27" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>159</v>
       </c>
@@ -2981,7 +3011,7 @@
       </c>
       <c r="J27" s="36"/>
     </row>
-    <row r="28" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
         <v>159</v>
       </c>
@@ -3003,21 +3033,21 @@
       </c>
       <c r="J28" s="36"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="E32" s="34"/>
       <c r="G32" s="42"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
     </row>
-    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="37" t="s">
         <v>32</v>
       </c>
@@ -3035,36 +3065,43 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B7" xr:uid="{71BDF466-626D-DA46-89A6-618460B87383}">
-      <formula1>Publishers</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{71BDF466-626D-DA46-89A6-618460B87383}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6:B7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3075,7 +3112,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3086,7 +3123,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3097,7 +3134,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3108,7 +3145,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3117,6 +3154,17 @@
       </c>
       <c r="C6" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3126,6 +3174,7 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{7C9EAC16-5214-429B-BD55-0ACFD949FAFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3137,16 +3186,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>127</v>
       </c>
@@ -3154,7 +3203,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -3162,7 +3211,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>129</v>
       </c>
@@ -3399,18 +3448,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3433,14 +3482,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{915D0155-BA4B-44F2-9111-0BC494AB9DE6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14FB0D8E-A90D-4B0C-ACC2-9EDC9E6A8195}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="97bb4d45-1042-4c49-a7f1-494cbdb4d63a"/>
@@ -3455,4 +3496,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{915D0155-BA4B-44F2-9111-0BC494AB9DE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>